<commit_message>
Commit Board and Card
</commit_message>
<xml_diff>
--- a/src/test/resources/config/DataTest.xlsx
+++ b/src/test/resources/config/DataTest.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trello Rest Assured\src\test\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9135B05C-895C-4F39-9546-EBC897D17D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC32CF9-94EF-4BB9-BEAB-3E897C562E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateACard" sheetId="2" r:id="rId1"/>
-    <sheet name="Create" sheetId="1" r:id="rId2"/>
+    <sheet name="Board" sheetId="1" r:id="rId1"/>
+    <sheet name="Card" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,32 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Kaka</t>
-  </si>
-  <si>
-    <t>Sale</t>
-  </si>
-  <si>
-    <t>Hona</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>job</t>
-  </si>
-  <si>
     <t>No.</t>
   </si>
   <si>
@@ -89,15 +68,45 @@
   </si>
   <si>
     <t>This is a bug</t>
+  </si>
+  <si>
+    <t>Create A Board Successfully</t>
+  </si>
+  <si>
+    <t>The new Chapter</t>
+  </si>
+  <si>
+    <t>Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book</t>
+  </si>
+  <si>
+    <t>Update A Board Successfully</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>[Updated] The new Chapter</t>
+  </si>
+  <si>
+    <t>[Updated] Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book</t>
+  </si>
+  <si>
+    <t>2023-03-29</t>
+  </si>
+  <si>
+    <t>[Updated] New Bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Updated] Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
+  </si>
+  <si>
+    <t>2023-03-30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -141,7 +150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -423,17 +432,125 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.296875" customWidth="1"/>
+    <col min="4" max="4" width="15.69921875" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
+    <col min="6" max="6" width="18.09765625" customWidth="1"/>
+    <col min="7" max="7" width="22.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9604356E-1A15-4209-9B72-022C3FA8FAE0}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.69921875" customWidth="1"/>
     <col min="2" max="2" width="36.59765625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="10.09765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.296875" customWidth="1"/>
     <col min="8" max="8" width="15.09765625" customWidth="1"/>
@@ -442,37 +559,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -480,22 +597,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3">
-        <v>45014</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
       </c>
       <c r="H2" s="2">
         <v>200</v>
@@ -508,11 +625,21 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -536,51 +663,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit checkList and checkItem
</commit_message>
<xml_diff>
--- a/src/test/resources/config/DataTest.xlsx
+++ b/src/test/resources/config/DataTest.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Trello Rest Assured\src\test\resources\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanapoto/Desktop/Trello-Rest-Assured-API/src/test/resources/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D81D10B-FEBA-45CD-906E-CE584424B251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE94C0A6-0EB6-1941-8C2B-11440E6CABB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Board" sheetId="1" r:id="rId1"/>
     <sheet name="ListColumn" sheetId="5" r:id="rId2"/>
     <sheet name="Card" sheetId="2" r:id="rId3"/>
     <sheet name="Attachment" sheetId="4" r:id="rId4"/>
+    <sheet name="CheckList" sheetId="6" r:id="rId5"/>
+    <sheet name="Stickers" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>name</t>
   </si>
@@ -145,6 +147,30 @@
   </si>
   <si>
     <t>src\\test\\resources\\config\\ImageTest.jpg</t>
+  </si>
+  <si>
+    <t>Create a CheckList successfully</t>
+  </si>
+  <si>
+    <t>This task should do:</t>
+  </si>
+  <si>
+    <t>Create a Stickers successfully</t>
+  </si>
+  <si>
+    <t>zIndex</t>
+  </si>
+  <si>
+    <t>rotate</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>image</t>
   </si>
 </sst>
 </file>
@@ -155,7 +181,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -163,7 +189,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -496,16 +522,16 @@
       <selection activeCell="G1" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.296875" customWidth="1"/>
-    <col min="4" max="4" width="15.69921875" customWidth="1"/>
-    <col min="5" max="5" width="19.69921875" customWidth="1"/>
-    <col min="6" max="6" width="18.19921875" customWidth="1"/>
-    <col min="7" max="7" width="22.19921875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -534,7 +560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -554,7 +580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -574,17 +600,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -602,14 +628,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="35.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.8984375" customWidth="1"/>
-    <col min="5" max="6" width="18.19921875" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="6" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -629,7 +655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -646,27 +672,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>37</v>
       </c>
@@ -684,19 +710,19 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.69921875" customWidth="1"/>
-    <col min="2" max="2" width="36.69921875" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.296875" customWidth="1"/>
-    <col min="8" max="8" width="15.19921875" customWidth="1"/>
-    <col min="9" max="9" width="18.796875" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -731,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -760,7 +786,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -785,7 +811,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -808,21 +834,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F29EB179-E607-934F-9CD0-3DAD35AB983F}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.69921875" customWidth="1"/>
-    <col min="2" max="2" width="36.69921875" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" customWidth="1"/>
-    <col min="7" max="7" width="18.796875" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -851,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -874,7 +900,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -897,7 +923,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -915,4 +941,177 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646EE2EA-E0CE-8D4B-9742-FDC94749ADB7}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2">
+        <v>200</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DD05CE-E76A-634E-9CCE-7E09EE143672}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2">
+        <v>50</v>
+      </c>
+      <c r="G2" s="2">
+        <v>50</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2">
+        <v>200</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>